<commit_message>
stable version (to Ivan)
</commit_message>
<xml_diff>
--- a/inclination data/vert (1m).xlsx
+++ b/inclination data/vert (1m).xlsx
@@ -347,7 +347,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -357,8 +357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A968" workbookViewId="0">
-      <selection activeCell="C1005" sqref="C1005"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B688" sqref="B688:B1007"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6383,7 +6383,7 @@
         <v>665</v>
       </c>
       <c r="B669">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
@@ -6392,7 +6392,7 @@
         <v>666</v>
       </c>
       <c r="B670">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.25">
@@ -6401,7 +6401,7 @@
         <v>667</v>
       </c>
       <c r="B671">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.25">
@@ -6410,7 +6410,7 @@
         <v>668</v>
       </c>
       <c r="B672">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.25">
@@ -6419,7 +6419,7 @@
         <v>669</v>
       </c>
       <c r="B673">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.25">
@@ -6428,7 +6428,7 @@
         <v>670</v>
       </c>
       <c r="B674">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.25">
@@ -6437,7 +6437,7 @@
         <v>671</v>
       </c>
       <c r="B675">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.25">
@@ -6446,7 +6446,7 @@
         <v>672</v>
       </c>
       <c r="B676">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.25">
@@ -6455,7 +6455,7 @@
         <v>673</v>
       </c>
       <c r="B677">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.25">
@@ -6464,7 +6464,7 @@
         <v>674</v>
       </c>
       <c r="B678">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.25">
@@ -6473,7 +6473,7 @@
         <v>675</v>
       </c>
       <c r="B679">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.25">
@@ -6482,7 +6482,7 @@
         <v>676</v>
       </c>
       <c r="B680">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.25">
@@ -6491,7 +6491,7 @@
         <v>677</v>
       </c>
       <c r="B681">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.25">
@@ -6500,7 +6500,7 @@
         <v>678</v>
       </c>
       <c r="B682">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.25">
@@ -6509,7 +6509,7 @@
         <v>679</v>
       </c>
       <c r="B683">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.25">
@@ -6518,7 +6518,7 @@
         <v>680</v>
       </c>
       <c r="B684">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.25">
@@ -6527,7 +6527,7 @@
         <v>681</v>
       </c>
       <c r="B685">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.25">
@@ -6536,7 +6536,7 @@
         <v>682</v>
       </c>
       <c r="B686">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.25">
@@ -6545,7 +6545,7 @@
         <v>683</v>
       </c>
       <c r="B687">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.25">
@@ -6554,7 +6554,7 @@
         <v>684</v>
       </c>
       <c r="B688">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.25">
@@ -6563,7 +6563,7 @@
         <v>685</v>
       </c>
       <c r="B689">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.25">
@@ -6572,7 +6572,7 @@
         <v>686</v>
       </c>
       <c r="B690">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.25">
@@ -6581,7 +6581,7 @@
         <v>687</v>
       </c>
       <c r="B691">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.25">
@@ -6590,7 +6590,7 @@
         <v>688</v>
       </c>
       <c r="B692">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.25">
@@ -6599,7 +6599,7 @@
         <v>689</v>
       </c>
       <c r="B693">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.25">
@@ -6608,7 +6608,7 @@
         <v>690</v>
       </c>
       <c r="B694">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.25">
@@ -6617,7 +6617,7 @@
         <v>691</v>
       </c>
       <c r="B695">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.25">
@@ -6626,7 +6626,7 @@
         <v>692</v>
       </c>
       <c r="B696">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.25">
@@ -6635,7 +6635,7 @@
         <v>693</v>
       </c>
       <c r="B697">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.25">
@@ -6644,7 +6644,7 @@
         <v>694</v>
       </c>
       <c r="B698">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.25">
@@ -6653,7 +6653,7 @@
         <v>695</v>
       </c>
       <c r="B699">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
@@ -6662,7 +6662,7 @@
         <v>696</v>
       </c>
       <c r="B700">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
@@ -6671,7 +6671,7 @@
         <v>697</v>
       </c>
       <c r="B701">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
@@ -6680,7 +6680,7 @@
         <v>698</v>
       </c>
       <c r="B702">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
@@ -6689,7 +6689,7 @@
         <v>699</v>
       </c>
       <c r="B703">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
@@ -6698,7 +6698,7 @@
         <v>700</v>
       </c>
       <c r="B704">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
@@ -6707,7 +6707,7 @@
         <v>701</v>
       </c>
       <c r="B705">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
@@ -6716,7 +6716,7 @@
         <v>702</v>
       </c>
       <c r="B706">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
@@ -6725,7 +6725,7 @@
         <v>703</v>
       </c>
       <c r="B707">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
@@ -6734,7 +6734,7 @@
         <v>704</v>
       </c>
       <c r="B708">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
@@ -6743,7 +6743,7 @@
         <v>705</v>
       </c>
       <c r="B709">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
@@ -6752,7 +6752,7 @@
         <v>706</v>
       </c>
       <c r="B710">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
@@ -6761,7 +6761,7 @@
         <v>707</v>
       </c>
       <c r="B711">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
@@ -6770,7 +6770,7 @@
         <v>708</v>
       </c>
       <c r="B712">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
@@ -6779,7 +6779,7 @@
         <v>709</v>
       </c>
       <c r="B713">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
@@ -6788,7 +6788,7 @@
         <v>710</v>
       </c>
       <c r="B714">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
@@ -6815,7 +6815,7 @@
         <v>713</v>
       </c>
       <c r="B717">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
@@ -6824,7 +6824,7 @@
         <v>714</v>
       </c>
       <c r="B718">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
@@ -6833,7 +6833,7 @@
         <v>715</v>
       </c>
       <c r="B719">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
@@ -6842,7 +6842,7 @@
         <v>716</v>
       </c>
       <c r="B720">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
@@ -6851,7 +6851,7 @@
         <v>717</v>
       </c>
       <c r="B721">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
@@ -6860,7 +6860,7 @@
         <v>718</v>
       </c>
       <c r="B722">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
@@ -6869,7 +6869,7 @@
         <v>719</v>
       </c>
       <c r="B723">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
@@ -6878,7 +6878,7 @@
         <v>720</v>
       </c>
       <c r="B724">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
@@ -6887,7 +6887,7 @@
         <v>721</v>
       </c>
       <c r="B725">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
@@ -6896,7 +6896,7 @@
         <v>722</v>
       </c>
       <c r="B726">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
@@ -6905,7 +6905,7 @@
         <v>723</v>
       </c>
       <c r="B727">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
@@ -6914,7 +6914,7 @@
         <v>724</v>
       </c>
       <c r="B728">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
@@ -6923,7 +6923,7 @@
         <v>725</v>
       </c>
       <c r="B729">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
@@ -6932,7 +6932,7 @@
         <v>726</v>
       </c>
       <c r="B730">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
@@ -6941,7 +6941,7 @@
         <v>727</v>
       </c>
       <c r="B731">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
@@ -6950,7 +6950,7 @@
         <v>728</v>
       </c>
       <c r="B732">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
@@ -6959,7 +6959,7 @@
         <v>729</v>
       </c>
       <c r="B733">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
@@ -6968,7 +6968,7 @@
         <v>730</v>
       </c>
       <c r="B734">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
@@ -6977,7 +6977,7 @@
         <v>731</v>
       </c>
       <c r="B735">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
@@ -6986,7 +6986,7 @@
         <v>732</v>
       </c>
       <c r="B736">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
@@ -6995,7 +6995,7 @@
         <v>733</v>
       </c>
       <c r="B737">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
@@ -7004,7 +7004,7 @@
         <v>734</v>
       </c>
       <c r="B738">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
@@ -7013,7 +7013,7 @@
         <v>735</v>
       </c>
       <c r="B739">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
@@ -7022,7 +7022,7 @@
         <v>736</v>
       </c>
       <c r="B740">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
@@ -7031,7 +7031,7 @@
         <v>737</v>
       </c>
       <c r="B741">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
@@ -7040,7 +7040,7 @@
         <v>738</v>
       </c>
       <c r="B742">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
@@ -7049,7 +7049,7 @@
         <v>739</v>
       </c>
       <c r="B743">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
@@ -7058,7 +7058,7 @@
         <v>740</v>
       </c>
       <c r="B744">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
@@ -7067,7 +7067,7 @@
         <v>741</v>
       </c>
       <c r="B745">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
@@ -7076,7 +7076,7 @@
         <v>742</v>
       </c>
       <c r="B746">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
@@ -7085,7 +7085,7 @@
         <v>743</v>
       </c>
       <c r="B747">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
@@ -7094,7 +7094,7 @@
         <v>744</v>
       </c>
       <c r="B748">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
@@ -7103,7 +7103,7 @@
         <v>745</v>
       </c>
       <c r="B749">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
@@ -7112,7 +7112,7 @@
         <v>746</v>
       </c>
       <c r="B750">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
@@ -7121,7 +7121,7 @@
         <v>747</v>
       </c>
       <c r="B751">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
@@ -7130,7 +7130,7 @@
         <v>748</v>
       </c>
       <c r="B752">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
@@ -7139,7 +7139,7 @@
         <v>749</v>
       </c>
       <c r="B753">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
@@ -7148,7 +7148,7 @@
         <v>750</v>
       </c>
       <c r="B754">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
@@ -7157,7 +7157,7 @@
         <v>751</v>
       </c>
       <c r="B755">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
@@ -7166,7 +7166,7 @@
         <v>752</v>
       </c>
       <c r="B756">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
@@ -7175,7 +7175,7 @@
         <v>753</v>
       </c>
       <c r="B757">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
@@ -7184,7 +7184,7 @@
         <v>754</v>
       </c>
       <c r="B758">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
@@ -7193,7 +7193,7 @@
         <v>755</v>
       </c>
       <c r="B759">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
@@ -7202,7 +7202,7 @@
         <v>756</v>
       </c>
       <c r="B760">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.25">
@@ -7211,7 +7211,7 @@
         <v>757</v>
       </c>
       <c r="B761">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.25">
@@ -7220,7 +7220,7 @@
         <v>758</v>
       </c>
       <c r="B762">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
@@ -7229,7 +7229,7 @@
         <v>759</v>
       </c>
       <c r="B763">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
@@ -7238,7 +7238,7 @@
         <v>760</v>
       </c>
       <c r="B764">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
@@ -7247,7 +7247,7 @@
         <v>761</v>
       </c>
       <c r="B765">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
@@ -7256,7 +7256,7 @@
         <v>762</v>
       </c>
       <c r="B766">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.25">
@@ -7265,7 +7265,7 @@
         <v>763</v>
       </c>
       <c r="B767">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.25">
@@ -7274,7 +7274,7 @@
         <v>764</v>
       </c>
       <c r="B768">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.25">
@@ -7283,7 +7283,7 @@
         <v>765</v>
       </c>
       <c r="B769">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.25">
@@ -7292,7 +7292,7 @@
         <v>766</v>
       </c>
       <c r="B770">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.25">
@@ -7301,7 +7301,7 @@
         <v>767</v>
       </c>
       <c r="B771">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
@@ -7310,7 +7310,7 @@
         <v>768</v>
       </c>
       <c r="B772">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
@@ -7319,7 +7319,7 @@
         <v>769</v>
       </c>
       <c r="B773">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
@@ -7328,7 +7328,7 @@
         <v>770</v>
       </c>
       <c r="B774">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
@@ -7337,7 +7337,7 @@
         <v>771</v>
       </c>
       <c r="B775">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.25">
@@ -7346,7 +7346,7 @@
         <v>772</v>
       </c>
       <c r="B776">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.25">
@@ -7355,7 +7355,7 @@
         <v>773</v>
       </c>
       <c r="B777">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
@@ -7364,7 +7364,7 @@
         <v>774</v>
       </c>
       <c r="B778">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
@@ -7373,7 +7373,7 @@
         <v>775</v>
       </c>
       <c r="B779">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.25">
@@ -7382,7 +7382,7 @@
         <v>776</v>
       </c>
       <c r="B780">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.25">
@@ -7391,7 +7391,7 @@
         <v>777</v>
       </c>
       <c r="B781">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.25">
@@ -7400,7 +7400,7 @@
         <v>778</v>
       </c>
       <c r="B782">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
@@ -7409,7 +7409,7 @@
         <v>779</v>
       </c>
       <c r="B783">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
@@ -7418,7 +7418,7 @@
         <v>780</v>
       </c>
       <c r="B784">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.25">
@@ -7427,7 +7427,7 @@
         <v>781</v>
       </c>
       <c r="B785">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.25">
@@ -7436,7 +7436,7 @@
         <v>782</v>
       </c>
       <c r="B786">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.25">
@@ -7445,7 +7445,7 @@
         <v>783</v>
       </c>
       <c r="B787">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
@@ -7454,7 +7454,7 @@
         <v>784</v>
       </c>
       <c r="B788">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
@@ -7463,7 +7463,7 @@
         <v>785</v>
       </c>
       <c r="B789">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.25">
@@ -7472,7 +7472,7 @@
         <v>786</v>
       </c>
       <c r="B790">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.25">
@@ -7481,7 +7481,7 @@
         <v>787</v>
       </c>
       <c r="B791">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.25">
@@ -7490,7 +7490,7 @@
         <v>788</v>
       </c>
       <c r="B792">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
@@ -7499,7 +7499,7 @@
         <v>789</v>
       </c>
       <c r="B793">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
@@ -7508,7 +7508,7 @@
         <v>790</v>
       </c>
       <c r="B794">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
@@ -7517,7 +7517,7 @@
         <v>791</v>
       </c>
       <c r="B795">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.25">
@@ -7526,7 +7526,7 @@
         <v>792</v>
       </c>
       <c r="B796">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.25">
@@ -7535,7 +7535,7 @@
         <v>793</v>
       </c>
       <c r="B797">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
@@ -7544,7 +7544,7 @@
         <v>794</v>
       </c>
       <c r="B798">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
@@ -7553,7 +7553,7 @@
         <v>795</v>
       </c>
       <c r="B799">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
@@ -7562,7 +7562,7 @@
         <v>796</v>
       </c>
       <c r="B800">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.25">
@@ -7571,7 +7571,7 @@
         <v>797</v>
       </c>
       <c r="B801">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.25">
@@ -7580,7 +7580,7 @@
         <v>798</v>
       </c>
       <c r="B802">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
@@ -7589,7 +7589,7 @@
         <v>799</v>
       </c>
       <c r="B803">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
@@ -7598,7 +7598,7 @@
         <v>800</v>
       </c>
       <c r="B804">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.25">
@@ -7607,7 +7607,7 @@
         <v>801</v>
       </c>
       <c r="B805">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.25">
@@ -7616,7 +7616,7 @@
         <v>802</v>
       </c>
       <c r="B806">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.25">
@@ -7625,7 +7625,7 @@
         <v>803</v>
       </c>
       <c r="B807">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.25">
@@ -7634,7 +7634,7 @@
         <v>804</v>
       </c>
       <c r="B808">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.25">
@@ -7643,7 +7643,7 @@
         <v>805</v>
       </c>
       <c r="B809">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.25">
@@ -7652,7 +7652,7 @@
         <v>806</v>
       </c>
       <c r="B810">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.25">
@@ -7661,7 +7661,7 @@
         <v>807</v>
       </c>
       <c r="B811">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.25">
@@ -7670,7 +7670,7 @@
         <v>808</v>
       </c>
       <c r="B812">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.25">
@@ -7679,7 +7679,7 @@
         <v>809</v>
       </c>
       <c r="B813">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.25">
@@ -7688,7 +7688,7 @@
         <v>810</v>
       </c>
       <c r="B814">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.25">
@@ -7697,7 +7697,7 @@
         <v>811</v>
       </c>
       <c r="B815">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.25">
@@ -7706,7 +7706,7 @@
         <v>812</v>
       </c>
       <c r="B816">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.25">
@@ -7715,7 +7715,7 @@
         <v>813</v>
       </c>
       <c r="B817">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.25">
@@ -7724,7 +7724,7 @@
         <v>814</v>
       </c>
       <c r="B818">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.25">
@@ -7733,7 +7733,7 @@
         <v>815</v>
       </c>
       <c r="B819">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.25">
@@ -7742,7 +7742,7 @@
         <v>816</v>
       </c>
       <c r="B820">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.25">
@@ -7751,7 +7751,7 @@
         <v>817</v>
       </c>
       <c r="B821">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.25">
@@ -7760,7 +7760,7 @@
         <v>818</v>
       </c>
       <c r="B822">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.25">
@@ -7769,7 +7769,7 @@
         <v>819</v>
       </c>
       <c r="B823">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.25">
@@ -7778,7 +7778,7 @@
         <v>820</v>
       </c>
       <c r="B824">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.25">
@@ -7787,7 +7787,7 @@
         <v>821</v>
       </c>
       <c r="B825">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.25">
@@ -7796,7 +7796,7 @@
         <v>822</v>
       </c>
       <c r="B826">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.25">
@@ -7805,7 +7805,7 @@
         <v>823</v>
       </c>
       <c r="B827">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.25">
@@ -7814,7 +7814,7 @@
         <v>824</v>
       </c>
       <c r="B828">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.25">
@@ -7823,7 +7823,7 @@
         <v>825</v>
       </c>
       <c r="B829">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.25">
@@ -7832,7 +7832,7 @@
         <v>826</v>
       </c>
       <c r="B830">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.25">
@@ -7841,7 +7841,7 @@
         <v>827</v>
       </c>
       <c r="B831">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.25">
@@ -7850,7 +7850,7 @@
         <v>828</v>
       </c>
       <c r="B832">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.25">
@@ -7859,7 +7859,7 @@
         <v>829</v>
       </c>
       <c r="B833">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.25">
@@ -7868,7 +7868,7 @@
         <v>830</v>
       </c>
       <c r="B834">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.25">
@@ -7877,7 +7877,7 @@
         <v>831</v>
       </c>
       <c r="B835">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.25">
@@ -7886,7 +7886,7 @@
         <v>832</v>
       </c>
       <c r="B836">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.25">
@@ -7895,7 +7895,7 @@
         <v>833</v>
       </c>
       <c r="B837">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.25">
@@ -7904,7 +7904,7 @@
         <v>834</v>
       </c>
       <c r="B838">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.25">
@@ -7913,7 +7913,7 @@
         <v>835</v>
       </c>
       <c r="B839">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.25">
@@ -7922,7 +7922,7 @@
         <v>836</v>
       </c>
       <c r="B840">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.25">
@@ -7931,7 +7931,7 @@
         <v>837</v>
       </c>
       <c r="B841">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.25">
@@ -7940,7 +7940,7 @@
         <v>838</v>
       </c>
       <c r="B842">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.25">
@@ -7949,7 +7949,7 @@
         <v>839</v>
       </c>
       <c r="B843">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.25">
@@ -7958,7 +7958,7 @@
         <v>840</v>
       </c>
       <c r="B844">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.25">
@@ -7967,7 +7967,7 @@
         <v>841</v>
       </c>
       <c r="B845">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.25">
@@ -7976,7 +7976,7 @@
         <v>842</v>
       </c>
       <c r="B846">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.25">
@@ -7985,7 +7985,7 @@
         <v>843</v>
       </c>
       <c r="B847">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.25">
@@ -7994,7 +7994,7 @@
         <v>844</v>
       </c>
       <c r="B848">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.25">
@@ -8003,7 +8003,7 @@
         <v>845</v>
       </c>
       <c r="B849">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.25">
@@ -8012,7 +8012,7 @@
         <v>846</v>
       </c>
       <c r="B850">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.25">
@@ -8021,7 +8021,7 @@
         <v>847</v>
       </c>
       <c r="B851">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.25">
@@ -8030,7 +8030,7 @@
         <v>848</v>
       </c>
       <c r="B852">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.25">
@@ -8039,7 +8039,7 @@
         <v>849</v>
       </c>
       <c r="B853">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.25">
@@ -8048,7 +8048,7 @@
         <v>850</v>
       </c>
       <c r="B854">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.25">
@@ -8057,7 +8057,7 @@
         <v>851</v>
       </c>
       <c r="B855">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.25">
@@ -8066,7 +8066,7 @@
         <v>852</v>
       </c>
       <c r="B856">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.25">
@@ -8075,7 +8075,7 @@
         <v>853</v>
       </c>
       <c r="B857">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.25">
@@ -8084,7 +8084,7 @@
         <v>854</v>
       </c>
       <c r="B858">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.25">
@@ -8093,7 +8093,7 @@
         <v>855</v>
       </c>
       <c r="B859">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.25">
@@ -8102,7 +8102,7 @@
         <v>856</v>
       </c>
       <c r="B860">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.25">
@@ -8111,7 +8111,7 @@
         <v>857</v>
       </c>
       <c r="B861">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.25">
@@ -8120,7 +8120,7 @@
         <v>858</v>
       </c>
       <c r="B862">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.25">
@@ -8129,7 +8129,7 @@
         <v>859</v>
       </c>
       <c r="B863">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.25">
@@ -8138,7 +8138,7 @@
         <v>860</v>
       </c>
       <c r="B864">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.25">
@@ -8147,7 +8147,7 @@
         <v>861</v>
       </c>
       <c r="B865">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.25">
@@ -8156,7 +8156,7 @@
         <v>862</v>
       </c>
       <c r="B866">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.25">
@@ -8165,7 +8165,7 @@
         <v>863</v>
       </c>
       <c r="B867">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.25">
@@ -8174,7 +8174,7 @@
         <v>864</v>
       </c>
       <c r="B868">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.25">
@@ -8183,7 +8183,7 @@
         <v>865</v>
       </c>
       <c r="B869">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.25">
@@ -8192,7 +8192,7 @@
         <v>866</v>
       </c>
       <c r="B870">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.25">
@@ -8201,7 +8201,7 @@
         <v>867</v>
       </c>
       <c r="B871">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.25">
@@ -8210,7 +8210,7 @@
         <v>868</v>
       </c>
       <c r="B872">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.25">
@@ -8219,7 +8219,7 @@
         <v>869</v>
       </c>
       <c r="B873">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.25">
@@ -8228,7 +8228,7 @@
         <v>870</v>
       </c>
       <c r="B874">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.25">
@@ -8237,7 +8237,7 @@
         <v>871</v>
       </c>
       <c r="B875">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.25">
@@ -8246,7 +8246,7 @@
         <v>872</v>
       </c>
       <c r="B876">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.25">
@@ -8255,7 +8255,7 @@
         <v>873</v>
       </c>
       <c r="B877">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.25">
@@ -8264,7 +8264,7 @@
         <v>874</v>
       </c>
       <c r="B878">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.25">
@@ -8273,7 +8273,7 @@
         <v>875</v>
       </c>
       <c r="B879">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.25">
@@ -8282,7 +8282,7 @@
         <v>876</v>
       </c>
       <c r="B880">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.25">
@@ -8291,7 +8291,7 @@
         <v>877</v>
       </c>
       <c r="B881">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.25">
@@ -8300,7 +8300,7 @@
         <v>878</v>
       </c>
       <c r="B882">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.25">
@@ -8309,7 +8309,7 @@
         <v>879</v>
       </c>
       <c r="B883">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.25">
@@ -8318,7 +8318,7 @@
         <v>880</v>
       </c>
       <c r="B884">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.25">
@@ -8327,7 +8327,7 @@
         <v>881</v>
       </c>
       <c r="B885">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.25">
@@ -8336,7 +8336,7 @@
         <v>882</v>
       </c>
       <c r="B886">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.25">
@@ -8345,7 +8345,7 @@
         <v>883</v>
       </c>
       <c r="B887">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.25">
@@ -8354,7 +8354,7 @@
         <v>884</v>
       </c>
       <c r="B888">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.25">
@@ -8363,7 +8363,7 @@
         <v>885</v>
       </c>
       <c r="B889">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.25">
@@ -8372,7 +8372,7 @@
         <v>886</v>
       </c>
       <c r="B890">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.25">
@@ -8381,7 +8381,7 @@
         <v>887</v>
       </c>
       <c r="B891">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.25">
@@ -8390,7 +8390,7 @@
         <v>888</v>
       </c>
       <c r="B892">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.25">
@@ -8399,7 +8399,7 @@
         <v>889</v>
       </c>
       <c r="B893">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.25">
@@ -8408,7 +8408,7 @@
         <v>890</v>
       </c>
       <c r="B894">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.25">
@@ -8417,7 +8417,7 @@
         <v>891</v>
       </c>
       <c r="B895">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.25">
@@ -8426,7 +8426,7 @@
         <v>892</v>
       </c>
       <c r="B896">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.25">
@@ -8435,7 +8435,7 @@
         <v>893</v>
       </c>
       <c r="B897">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.25">
@@ -8444,7 +8444,7 @@
         <v>894</v>
       </c>
       <c r="B898">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.25">
@@ -8453,7 +8453,7 @@
         <v>895</v>
       </c>
       <c r="B899">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.25">
@@ -8462,7 +8462,7 @@
         <v>896</v>
       </c>
       <c r="B900">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.25">
@@ -8471,7 +8471,7 @@
         <v>897</v>
       </c>
       <c r="B901">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.25">
@@ -8480,7 +8480,7 @@
         <v>898</v>
       </c>
       <c r="B902">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.25">
@@ -8489,7 +8489,7 @@
         <v>899</v>
       </c>
       <c r="B903">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.25">
@@ -8498,7 +8498,7 @@
         <v>900</v>
       </c>
       <c r="B904">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.25">
@@ -8507,7 +8507,7 @@
         <v>901</v>
       </c>
       <c r="B905">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.25">
@@ -8516,7 +8516,7 @@
         <v>902</v>
       </c>
       <c r="B906">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.25">
@@ -8525,7 +8525,7 @@
         <v>903</v>
       </c>
       <c r="B907">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.25">
@@ -8534,7 +8534,7 @@
         <v>904</v>
       </c>
       <c r="B908">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.25">
@@ -8543,7 +8543,7 @@
         <v>905</v>
       </c>
       <c r="B909">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.25">
@@ -8552,7 +8552,7 @@
         <v>906</v>
       </c>
       <c r="B910">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.25">
@@ -8561,7 +8561,7 @@
         <v>907</v>
       </c>
       <c r="B911">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.25">
@@ -8570,7 +8570,7 @@
         <v>908</v>
       </c>
       <c r="B912">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.25">
@@ -8579,7 +8579,7 @@
         <v>909</v>
       </c>
       <c r="B913">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.25">
@@ -8588,7 +8588,7 @@
         <v>910</v>
       </c>
       <c r="B914">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.25">
@@ -8597,7 +8597,7 @@
         <v>911</v>
       </c>
       <c r="B915">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.25">
@@ -8606,7 +8606,7 @@
         <v>912</v>
       </c>
       <c r="B916">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.25">
@@ -8615,7 +8615,7 @@
         <v>913</v>
       </c>
       <c r="B917">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.25">
@@ -8624,7 +8624,7 @@
         <v>914</v>
       </c>
       <c r="B918">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.25">
@@ -8633,7 +8633,7 @@
         <v>915</v>
       </c>
       <c r="B919">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.25">
@@ -8642,7 +8642,7 @@
         <v>916</v>
       </c>
       <c r="B920">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.25">
@@ -8651,7 +8651,7 @@
         <v>917</v>
       </c>
       <c r="B921">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.25">
@@ -8660,7 +8660,7 @@
         <v>918</v>
       </c>
       <c r="B922">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.25">
@@ -8669,7 +8669,7 @@
         <v>919</v>
       </c>
       <c r="B923">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.25">
@@ -8678,7 +8678,7 @@
         <v>920</v>
       </c>
       <c r="B924">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.25">
@@ -8687,7 +8687,7 @@
         <v>921</v>
       </c>
       <c r="B925">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.25">
@@ -8696,7 +8696,7 @@
         <v>922</v>
       </c>
       <c r="B926">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.25">
@@ -8705,7 +8705,7 @@
         <v>923</v>
       </c>
       <c r="B927">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.25">
@@ -8714,7 +8714,7 @@
         <v>924</v>
       </c>
       <c r="B928">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.25">
@@ -8723,7 +8723,7 @@
         <v>925</v>
       </c>
       <c r="B929">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.25">
@@ -8732,7 +8732,7 @@
         <v>926</v>
       </c>
       <c r="B930">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.25">
@@ -8741,7 +8741,7 @@
         <v>927</v>
       </c>
       <c r="B931">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.25">
@@ -8750,7 +8750,7 @@
         <v>928</v>
       </c>
       <c r="B932">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.25">
@@ -8759,7 +8759,7 @@
         <v>929</v>
       </c>
       <c r="B933">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.25">
@@ -8768,7 +8768,7 @@
         <v>930</v>
       </c>
       <c r="B934">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.25">
@@ -8777,7 +8777,7 @@
         <v>931</v>
       </c>
       <c r="B935">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.25">
@@ -8786,7 +8786,7 @@
         <v>932</v>
       </c>
       <c r="B936">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.25">
@@ -8795,7 +8795,7 @@
         <v>933</v>
       </c>
       <c r="B937">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.25">
@@ -8804,7 +8804,7 @@
         <v>934</v>
       </c>
       <c r="B938">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.25">
@@ -8813,7 +8813,7 @@
         <v>935</v>
       </c>
       <c r="B939">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.25">
@@ -8822,7 +8822,7 @@
         <v>936</v>
       </c>
       <c r="B940">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.25">
@@ -8831,7 +8831,7 @@
         <v>937</v>
       </c>
       <c r="B941">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.25">
@@ -8840,7 +8840,7 @@
         <v>938</v>
       </c>
       <c r="B942">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.25">
@@ -8849,7 +8849,7 @@
         <v>939</v>
       </c>
       <c r="B943">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.25">
@@ -8858,7 +8858,7 @@
         <v>940</v>
       </c>
       <c r="B944">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.25">
@@ -8867,7 +8867,7 @@
         <v>941</v>
       </c>
       <c r="B945">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.25">
@@ -8876,7 +8876,7 @@
         <v>942</v>
       </c>
       <c r="B946">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.25">
@@ -8885,7 +8885,7 @@
         <v>943</v>
       </c>
       <c r="B947">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.25">
@@ -8894,7 +8894,7 @@
         <v>944</v>
       </c>
       <c r="B948">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.25">
@@ -8903,7 +8903,7 @@
         <v>945</v>
       </c>
       <c r="B949">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.25">
@@ -8912,7 +8912,7 @@
         <v>946</v>
       </c>
       <c r="B950">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.25">
@@ -8921,7 +8921,7 @@
         <v>947</v>
       </c>
       <c r="B951">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.25">
@@ -8930,7 +8930,7 @@
         <v>948</v>
       </c>
       <c r="B952">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.25">
@@ -8939,7 +8939,7 @@
         <v>949</v>
       </c>
       <c r="B953">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.25">
@@ -8948,7 +8948,7 @@
         <v>950</v>
       </c>
       <c r="B954">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.25">
@@ -8957,7 +8957,7 @@
         <v>951</v>
       </c>
       <c r="B955">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.25">
@@ -8966,7 +8966,7 @@
         <v>952</v>
       </c>
       <c r="B956">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.25">
@@ -8975,7 +8975,7 @@
         <v>953</v>
       </c>
       <c r="B957">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.25">
@@ -8984,7 +8984,7 @@
         <v>954</v>
       </c>
       <c r="B958">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.25">
@@ -8993,7 +8993,7 @@
         <v>955</v>
       </c>
       <c r="B959">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.25">
@@ -9002,7 +9002,7 @@
         <v>956</v>
       </c>
       <c r="B960">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.25">
@@ -9011,7 +9011,7 @@
         <v>957</v>
       </c>
       <c r="B961">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.25">
@@ -9020,7 +9020,7 @@
         <v>958</v>
       </c>
       <c r="B962">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.25">
@@ -9029,7 +9029,7 @@
         <v>959</v>
       </c>
       <c r="B963">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.25">
@@ -9038,7 +9038,7 @@
         <v>960</v>
       </c>
       <c r="B964">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.25">
@@ -9047,7 +9047,7 @@
         <v>961</v>
       </c>
       <c r="B965">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.25">
@@ -9056,7 +9056,7 @@
         <v>962</v>
       </c>
       <c r="B966">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.25">
@@ -9065,7 +9065,7 @@
         <v>963</v>
       </c>
       <c r="B967">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.25">
@@ -9074,7 +9074,7 @@
         <v>964</v>
       </c>
       <c r="B968">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.25">
@@ -9083,7 +9083,7 @@
         <v>965</v>
       </c>
       <c r="B969">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.25">
@@ -9092,7 +9092,7 @@
         <v>966</v>
       </c>
       <c r="B970">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.25">
@@ -9101,7 +9101,7 @@
         <v>967</v>
       </c>
       <c r="B971">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.25">
@@ -9110,7 +9110,7 @@
         <v>968</v>
       </c>
       <c r="B972">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.25">
@@ -9119,7 +9119,7 @@
         <v>969</v>
       </c>
       <c r="B973">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.25">
@@ -9128,7 +9128,7 @@
         <v>970</v>
       </c>
       <c r="B974">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.25">
@@ -9137,7 +9137,7 @@
         <v>971</v>
       </c>
       <c r="B975">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.25">
@@ -9146,7 +9146,7 @@
         <v>972</v>
       </c>
       <c r="B976">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.25">
@@ -9155,7 +9155,7 @@
         <v>973</v>
       </c>
       <c r="B977">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.25">
@@ -9164,7 +9164,7 @@
         <v>974</v>
       </c>
       <c r="B978">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.25">
@@ -9173,7 +9173,7 @@
         <v>975</v>
       </c>
       <c r="B979">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.25">
@@ -9182,7 +9182,7 @@
         <v>976</v>
       </c>
       <c r="B980">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.25">
@@ -9191,7 +9191,7 @@
         <v>977</v>
       </c>
       <c r="B981">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.25">
@@ -9200,7 +9200,7 @@
         <v>978</v>
       </c>
       <c r="B982">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.25">
@@ -9209,7 +9209,7 @@
         <v>979</v>
       </c>
       <c r="B983">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.25">
@@ -9218,7 +9218,7 @@
         <v>980</v>
       </c>
       <c r="B984">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.25">
@@ -9227,7 +9227,7 @@
         <v>981</v>
       </c>
       <c r="B985">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.25">
@@ -9236,7 +9236,7 @@
         <v>982</v>
       </c>
       <c r="B986">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.25">
@@ -9245,7 +9245,7 @@
         <v>983</v>
       </c>
       <c r="B987">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.25">
@@ -9254,7 +9254,7 @@
         <v>984</v>
       </c>
       <c r="B988">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.25">
@@ -9263,7 +9263,7 @@
         <v>985</v>
       </c>
       <c r="B989">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.25">
@@ -9272,7 +9272,7 @@
         <v>986</v>
       </c>
       <c r="B990">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.25">
@@ -9281,7 +9281,7 @@
         <v>987</v>
       </c>
       <c r="B991">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.25">
@@ -9290,7 +9290,7 @@
         <v>988</v>
       </c>
       <c r="B992">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.25">
@@ -9299,7 +9299,7 @@
         <v>989</v>
       </c>
       <c r="B993">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.25">
@@ -9308,7 +9308,7 @@
         <v>990</v>
       </c>
       <c r="B994">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.25">
@@ -9317,7 +9317,7 @@
         <v>991</v>
       </c>
       <c r="B995">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.25">
@@ -9326,7 +9326,7 @@
         <v>992</v>
       </c>
       <c r="B996">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.25">
@@ -9335,7 +9335,7 @@
         <v>993</v>
       </c>
       <c r="B997">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>